<commit_message>
perbaikan agar seperti cat
</commit_message>
<xml_diff>
--- a/uploads/import/format/mahasiswa.xlsx
+++ b/uploads/import/format/mahasiswa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WEB_APP\ALIAS_WWW\oltest\uploads\import\format\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WEB_APP\ALIAS_WWW\ujianundip\uploads\import\format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6788C11-707A-4AFB-A805-1B06488380F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD51D372-72EC-45C6-BE86-2F77E8BD7892}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>L/P</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>NIK (BOLEH DIAWALI TANDA ' AGAR TIDAK BERMASALAH)</t>
+  </si>
+  <si>
+    <t>NO BILLKEY</t>
   </si>
 </sst>
 </file>
@@ -431,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -443,13 +446,15 @@
     <col min="3" max="3" width="45.625" style="8" customWidth="1"/>
     <col min="4" max="4" width="36.625" style="3" customWidth="1"/>
     <col min="5" max="5" width="36.625" style="6" customWidth="1"/>
-    <col min="6" max="7" width="27.625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="7" style="3" customWidth="1"/>
-    <col min="9" max="9" width="32.75" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="2"/>
+    <col min="6" max="6" width="27.625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="36.625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="27.625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="7" style="3" customWidth="1"/>
+    <col min="10" max="10" width="32.75" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -469,41 +474,44 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="7"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="4"/>
+      <c r="H2" s="5"/>
       <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="7"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="4"/>
+      <c r="H3" s="5"/>
       <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="7"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="4"/>
+      <c r="H4" s="5"/>
       <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
perbaikan smt dan masa berlaku sertifikat
</commit_message>
<xml_diff>
--- a/uploads/import/format/mahasiswa.xlsx
+++ b/uploads/import/format/mahasiswa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WEB_APP\ALIAS_WWW\ujianundip\uploads\import\format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F81CB82-6088-4D23-B66A-22E23BFAF57B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61700F6-9BD2-4E60-B0CD-F1F5AEC771C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>L/P</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>TAHUN</t>
+  </si>
+  <si>
+    <t>SMT</t>
   </si>
 </sst>
 </file>
@@ -459,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -474,12 +477,12 @@
     <col min="6" max="6" width="7" style="3" customWidth="1"/>
     <col min="7" max="7" width="27.625" style="3" customWidth="1"/>
     <col min="8" max="8" width="36.625" style="3" customWidth="1"/>
-    <col min="9" max="14" width="27.625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="32.75" style="3" customWidth="1"/>
-    <col min="16" max="16384" width="9" style="2"/>
+    <col min="9" max="15" width="27.625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="32.75" style="3" customWidth="1"/>
+    <col min="17" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -520,13 +523,16 @@
         <v>13</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="7"/>
@@ -538,9 +544,10 @@
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
-      <c r="O2" s="4"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="4"/>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="7"/>
@@ -552,9 +559,10 @@
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
-      <c r="O3" s="4"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="4"/>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:16">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="7"/>
@@ -566,7 +574,8 @@
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
-      <c r="O4" s="4"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="4"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>